<commit_message>
Bab 3 Analisis Grafik sensor Accelero dengan Gryo rotation vector masih ragu
Ada tambahan kode program dari aplikasi perekam sensornya
</commit_message>
<xml_diff>
--- a/doc/Data Pengujian Sensor/Kiri Atas/sensorRecord-10-28-2016-50547-PM(Kiri atas Mengangguk).xlsx
+++ b/doc/Data Pengujian Sensor/Kiri Atas/sensorRecord-10-28-2016-50547-PM(Kiri atas Mengangguk).xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ega Prianto\Documents\GitHub\DevelopWorkspace\Skripsi\doc\Data Pengujian\Kiri Atas\Ko Wych\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Ega Prianto\Documents\GitHub\DevelopWorkspace\Skripsi\doc\Data Pengujian Sensor\Kiri Atas\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="450" windowWidth="20490" windowHeight="7890"/>
+    <workbookView xWindow="0" yWindow="900" windowWidth="20490" windowHeight="7890"/>
   </bookViews>
   <sheets>
     <sheet name="sensorRecord-10-28-2016-50547-P" sheetId="1" r:id="rId1"/>
@@ -34,9 +34,6 @@
   </si>
   <si>
     <t>z</t>
-  </si>
-  <si>
-    <t>Gyroscope</t>
   </si>
   <si>
     <t>Geomagnetic Rotation</t>
@@ -67,6 +64,9 @@
   </si>
   <si>
     <t>Running Time : 2465ms</t>
+  </si>
+  <si>
+    <t>s</t>
   </si>
 </sst>
 </file>
@@ -3076,11 +3076,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="609357136"/>
-        <c:axId val="609353216"/>
+        <c:axId val="672590896"/>
+        <c:axId val="672589776"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="609357136"/>
+        <c:axId val="672590896"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3137,12 +3137,12 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609353216"/>
+        <c:crossAx val="672589776"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="609353216"/>
+        <c:axId val="672589776"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3199,7 +3199,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="609357136"/>
+        <c:crossAx val="672590896"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5745,11 +5745,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="613940112"/>
-        <c:axId val="613949072"/>
+        <c:axId val="612444720"/>
+        <c:axId val="612445840"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="613940112"/>
+        <c:axId val="612444720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5806,12 +5806,12 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613949072"/>
+        <c:crossAx val="612445840"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="613949072"/>
+        <c:axId val="612445840"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -5868,7 +5868,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613940112"/>
+        <c:crossAx val="612444720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -5964,7 +5964,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8468,11 +8467,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="613951312"/>
-        <c:axId val="613951872"/>
+        <c:axId val="133579696"/>
+        <c:axId val="133581376"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="613951312"/>
+        <c:axId val="133579696"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8529,12 +8528,12 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613951872"/>
+        <c:crossAx val="133581376"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="613951872"/>
+        <c:axId val="133581376"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -8591,7 +8590,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="613951312"/>
+        <c:crossAx val="133579696"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -8605,7 +8604,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -8687,7 +8685,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12011,11 +12008,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="664369472"/>
-        <c:axId val="664370032"/>
+        <c:axId val="612277936"/>
+        <c:axId val="614476720"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="664369472"/>
+        <c:axId val="612277936"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12072,12 +12069,12 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664370032"/>
+        <c:crossAx val="614476720"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="664370032"/>
+        <c:axId val="614476720"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -12134,7 +12131,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="664369472"/>
+        <c:crossAx val="612277936"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -12148,7 +12145,6 @@
     </c:plotArea>
     <c:legend>
       <c:legendPos val="b"/>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -15554,11 +15550,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="606947136"/>
-        <c:axId val="606945456"/>
+        <c:axId val="678006448"/>
+        <c:axId val="678007008"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="606947136"/>
+        <c:axId val="678006448"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15615,12 +15611,12 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="606945456"/>
+        <c:crossAx val="678007008"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="606945456"/>
+        <c:axId val="678007008"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -15677,7 +15673,7 @@
             <a:endParaRPr lang="id-ID"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="606947136"/>
+        <c:crossAx val="678006448"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -18958,8 +18954,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F656"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A636" workbookViewId="0">
-      <selection activeCell="A654" sqref="A654:C656"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="A130" sqref="A130"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -20749,7 +20745,7 @@
     </row>
     <row r="130" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A130" t="s">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="131" spans="1:4" x14ac:dyDescent="0.25">
@@ -22532,7 +22528,7 @@
     </row>
     <row r="259" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A259" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="260" spans="1:4" x14ac:dyDescent="0.25">
@@ -24357,7 +24353,7 @@
     </row>
     <row r="391" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A391" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="392" spans="1:6" x14ac:dyDescent="0.25">
@@ -24365,19 +24361,19 @@
         <v>1</v>
       </c>
       <c r="B392" t="s">
+        <v>7</v>
+      </c>
+      <c r="C392" t="s">
         <v>8</v>
       </c>
-      <c r="C392" t="s">
+      <c r="D392" t="s">
         <v>9</v>
       </c>
-      <c r="D392" t="s">
+      <c r="E392" t="s">
         <v>10</v>
       </c>
-      <c r="E392" t="s">
+      <c r="F392" t="s">
         <v>11</v>
-      </c>
-      <c r="F392" t="s">
-        <v>12</v>
       </c>
     </row>
     <row r="393" spans="1:6" x14ac:dyDescent="0.25">
@@ -26962,7 +26958,7 @@
     </row>
     <row r="523" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A523" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
     </row>
     <row r="524" spans="1:6" x14ac:dyDescent="0.25">
@@ -26979,7 +26975,7 @@
         <v>4</v>
       </c>
       <c r="E524" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
     </row>
     <row r="525" spans="1:6" x14ac:dyDescent="0.25">
@@ -29177,7 +29173,7 @@
     </row>
     <row r="656" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A656" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
   </sheetData>

</xml_diff>